<commit_message>
interessentanalyse + usecase color added
</commit_message>
<xml_diff>
--- a/Analysis/Interessentanalyse.xlsx
+++ b/Analysis/Interessentanalyse.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas Mørch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\iCloudDrive\eclipse\flextur\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,22 +119,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -150,23 +176,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A2:E7" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A2:E7" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A2:E7"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Interessentanalyse - Flextur"/>
-    <tableColumn id="2" name="Ønsker" dataDxfId="0"/>
-    <tableColumn id="3" name="Behov"/>
-    <tableColumn id="4" name="Krav"/>
-    <tableColumn id="5" name="Overvejelser"/>
+    <tableColumn id="1" name="Interessentanalyse - Flextur" dataDxfId="0"/>
+    <tableColumn id="2" name="Ønsker" dataDxfId="1"/>
+    <tableColumn id="3" name="Behov" dataDxfId="5"/>
+    <tableColumn id="4" name="Krav" dataDxfId="4"/>
+    <tableColumn id="5" name="Overvejelser" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -276,7 +302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,19 +455,19 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -457,8 +483,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -474,8 +500,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -491,27 +517,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
       <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Intressent analyse opdateret og tilføjet i visions dokument
</commit_message>
<xml_diff>
--- a/Analysis/Interessentanalyse.xlsx
+++ b/Analysis/Interessentanalyse.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\iCloudDrive\eclipse\flextur\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas Mørch\Dropbox\Eclipse Workspace\flextur\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -29,15 +29,6 @@
     <t>Interessentanalyse - Flextur</t>
   </si>
   <si>
-    <t>Brugere</t>
-  </si>
-  <si>
-    <t>Kunde</t>
-  </si>
-  <si>
-    <t>Lovgivere</t>
-  </si>
-  <si>
     <t>Ønsker</t>
   </si>
   <si>
@@ -56,18 +47,12 @@
     <t>Systemet skal eksekveres hurtigt, men det skal være meget intuitivt for brugeren.</t>
   </si>
   <si>
-    <t>Da en større del af brugerene af sådan et system vil være ældre eller handicappede skal brugergrænsefladen være simpel og nem at finde rundt i.</t>
-  </si>
-  <si>
     <t>Nogle brugere har ikke adgang til smartphone appen, og ringer derfor direkte til MidtTrafik. En pc baseret løsning er ønsket af MidtTrafik.</t>
   </si>
   <si>
     <t>Systemet skal behandle data sikkert, og MidtTrafik skal også kunne bruge systemet til at se en oversigt af bestillinger lavet af brugere, samt godkende og tildele biler til disse.</t>
   </si>
   <si>
-    <t>I tilfælde af at potentiele brugere stadig kontakter MidtTrafik telefonisk for at bestille Flexture, så vil det være logisk at MidtTrafiks side af systemet også kan bruges til at registrere kørsler.</t>
-  </si>
-  <si>
     <t>MidtTrafik ønsker at både tilbyde sine brugere en bedre service angående bestilling af Flextur, men også at nedbringe belastningen af deres telefon support.</t>
   </si>
   <si>
@@ -77,19 +62,34 @@
     <t>At alle personfølsomme data behandles sikkert</t>
   </si>
   <si>
-    <t>Da vi som udviklere ikke er godkendt til at benytte CPR registret, falder denne Intressent uden for betydning af denne analyse.</t>
-  </si>
-  <si>
-    <t>Pengeinstitutet har behov for at brugerens bestilling og betaling foregår sikkert</t>
-  </si>
-  <si>
-    <t>Pengeinstitutet</t>
+    <t>Datatilsynet</t>
+  </si>
+  <si>
+    <t>MidtTrafik</t>
+  </si>
+  <si>
+    <t>MidtTrafiks kunder</t>
+  </si>
+  <si>
+    <t>Pengeinstituttet</t>
+  </si>
+  <si>
+    <t>Pengeinstituttet har behov for at brugerens bestilling og betaling foregår sikkert</t>
+  </si>
+  <si>
+    <t>Da en større del af brugerne af sådan et system vil være ældre eller handicappede skal brugergrænsefladen være simpel og nem at finde rundt i.</t>
+  </si>
+  <si>
+    <t>I tilfælde af at potentielle brugere stadig kontakter MidtTrafik telefonisk for at bestille Flexture, så vil det være logisk at MidtTrafiks side af systemet også kan bruges til at registrere kørsler.</t>
+  </si>
+  <si>
+    <t>Da vi som udviklere ikke er godkendt til at benytte CPR registret, falder denne Interessent uden for betydning af denne analyse.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,10 +145,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -157,7 +154,10 @@
       <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -176,23 +176,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A2:E7" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A2:E7" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A2:E7"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Interessentanalyse - Flextur" dataDxfId="0"/>
-    <tableColumn id="2" name="Ønsker" dataDxfId="1"/>
-    <tableColumn id="3" name="Behov" dataDxfId="5"/>
-    <tableColumn id="4" name="Krav" dataDxfId="4"/>
-    <tableColumn id="5" name="Overvejelser" dataDxfId="3"/>
+    <tableColumn id="1" name="Interessentanalyse - Flextur" dataDxfId="4"/>
+    <tableColumn id="2" name="Ønsker" dataDxfId="3"/>
+    <tableColumn id="3" name="Behov" dataDxfId="2"/>
+    <tableColumn id="4" name="Krav" dataDxfId="1"/>
+    <tableColumn id="5" name="Overvejelser" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -302,7 +302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,90 +458,90 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" style="4" customWidth="1"/>
-    <col min="2" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>

</xml_diff>

<commit_message>
Interessent analyse samt figur
</commit_message>
<xml_diff>
--- a/Analysis/Interessentanalyse.xlsx
+++ b/Analysis/Interessentanalyse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Interessentanalyse - Flextur</t>
   </si>
@@ -69,12 +69,6 @@
   </si>
   <si>
     <t>MidtTrafiks kunder</t>
-  </si>
-  <si>
-    <t>Pengeinstituttet</t>
-  </si>
-  <si>
-    <t>Pengeinstituttet har behov for at brugerens bestilling og betaling foregår sikkert</t>
   </si>
   <si>
     <t>Da en større del af brugerne af sådan et system vil være ældre eller handicappede skal brugergrænsefladen være simpel og nem at finde rundt i.</t>
@@ -455,7 +449,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -514,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -527,17 +521,13 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>

</xml_diff>

<commit_message>
intressent analyse opdateret + visions dokument
</commit_message>
<xml_diff>
--- a/Analysis/Interessentanalyse.xlsx
+++ b/Analysis/Interessentanalyse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Interessentanalyse - Flextur</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Datatilsynet</t>
   </si>
   <si>
-    <t>MidtTrafik</t>
-  </si>
-  <si>
     <t>MidtTrafiks kunder</t>
   </si>
   <si>
@@ -78,6 +75,24 @@
   </si>
   <si>
     <t>Da vi som udviklere ikke er godkendt til at benytte CPR registret, falder denne Interessent uden for betydning af denne analyse.</t>
+  </si>
+  <si>
+    <t>MidtTrafik (selskab)</t>
+  </si>
+  <si>
+    <t>MidtTrafik (bestillingsmodtagelse)</t>
+  </si>
+  <si>
+    <t>Et system der kan hjælpe med at nedsætte behovet for telefonisk bestilling.</t>
+  </si>
+  <si>
+    <t>At systemet er relativt nemt at sætte sig ind i så der ikker er nogen længere oplærings periode.</t>
+  </si>
+  <si>
+    <t>Systemet skal køre hurtigt, men også stabilt.</t>
+  </si>
+  <si>
+    <t>De menige ansatte som skal betjene den administrative side af systemet er ikke nødvendigvis særlig IT kyndige, derfor lægges der vægt på brugervenlighed også i denne del</t>
   </si>
 </sst>
 </file>
@@ -170,8 +185,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A2:E7" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A2:E6" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Interessentanalyse - Flextur" dataDxfId="4"/>
     <tableColumn id="2" name="Ønsker" dataDxfId="3"/>
@@ -446,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="A2:E5"/>
+      <selection activeCell="E6" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +494,7 @@
     </row>
     <row r="3" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -491,52 +506,55 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>